<commit_message>
develloped the file upload show icon
</commit_message>
<xml_diff>
--- a/php files/Questions.xlsx
+++ b/php files/Questions.xlsx
@@ -15,7 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+  <si>
+    <t>Start write your questions from here</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -353,7 +357,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -361,9 +365,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1">
-        <v>272</v>
+        <v>283</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>